<commit_message>
Updated my status and the Project Plan
</commit_message>
<xml_diff>
--- a/Documentation/WeeklyStatus_Jacob.xlsx
+++ b/Documentation/WeeklyStatus_Jacob.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="34400" windowHeight="22600" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="34400" windowHeight="22600" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="7-2-13" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="26">
   <si>
     <t>Date:</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -107,10 +107,6 @@
   </si>
   <si>
     <t>Time Spent</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Project Plan Assistance</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -502,7 +498,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -552,7 +548,7 @@
         <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
@@ -629,12 +625,12 @@
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" s="1">
         <v>39995</v>
@@ -649,10 +645,11 @@
         <v>2.5</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -665,10 +662,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -688,9 +685,6 @@
       <c r="E1" t="s">
         <v>15</v>
       </c>
-      <c r="F1">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
@@ -717,7 +711,7 @@
         <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
@@ -743,22 +737,17 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1">
-        <v>39995</v>
-      </c>
-      <c r="C4" s="1">
-        <v>40054</v>
-      </c>
+        <v>39997</v>
+      </c>
+      <c r="C4" s="1"/>
       <c r="D4" s="2">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="E4">
-        <v>2</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
+        <v>0.25</v>
       </c>
       <c r="H4" t="s">
         <v>20</v>
@@ -780,38 +769,11 @@
       </c>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="1">
-        <v>39997</v>
-      </c>
+      <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="2">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="A6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="1">
-        <v>39995</v>
-      </c>
-      <c r="C6" s="1">
-        <v>39995</v>
-      </c>
-      <c r="D6" s="2">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>2.5</v>
-      </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
Update test ssh project and status
</commit_message>
<xml_diff>
--- a/Documentation/WeeklyStatus_Jacob.xlsx
+++ b/Documentation/WeeklyStatus_Jacob.xlsx
@@ -724,6 +724,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -1003,6 +1004,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -1018,7 +1020,7 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1124,7 +1126,7 @@
         <v>40066</v>
       </c>
       <c r="D5" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -1138,13 +1140,14 @@
         <v>40069</v>
       </c>
       <c r="D6" s="2">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="E6">
-        <v>4</v>
+        <v>6.5</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
Updated Final Phase 1 code folder
</commit_message>
<xml_diff>
--- a/Documentation/WeeklyStatus_Jacob.xlsx
+++ b/Documentation/WeeklyStatus_Jacob.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="50">
   <si>
     <t>Date:</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -222,10 +222,6 @@
   </si>
   <si>
     <t>Project Report</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>started at 1:30</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -233,11 +229,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
   </numFmts>
@@ -1182,6 +1174,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -1302,6 +1295,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -1317,7 +1311,7 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1430,11 +1424,12 @@
       <c r="D6" s="2">
         <v>0.1</v>
       </c>
-      <c r="F6" t="s">
-        <v>50</v>
+      <c r="E6">
+        <v>3.5</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
Document updates and additions
Updated my status. Added Phase 2 plan, task spreadsheet and agenda for
the meeting Monday.
</commit_message>
<xml_diff>
--- a/Documentation/WeeklyStatus_Jacob.xlsx
+++ b/Documentation/WeeklyStatus_Jacob.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\4049dahleej\Documents\GitHub\EmbeddedSystems\Documentation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="34400" windowHeight="22600" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="34395" windowHeight="22605" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="9-2-13" sheetId="1" r:id="rId1"/>
@@ -13,7 +18,7 @@
     <sheet name="9-23-13" sheetId="4" r:id="rId4"/>
     <sheet name="9-30-13" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="130407" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -23,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="51">
   <si>
     <t>Date:</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -223,17 +228,20 @@
   <si>
     <t>Project Report</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Project Plan 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -274,6 +282,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -596,20 +612,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="2"/>
+    <col min="3" max="3" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.75" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -624,7 +640,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -635,7 +651,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -673,7 +689,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -711,7 +727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -729,7 +745,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -761,20 +777,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="3" width="10.7109375" style="3"/>
-    <col min="4" max="4" width="10.7109375" style="2"/>
+    <col min="2" max="3" width="10.75" style="3"/>
+    <col min="4" max="4" width="10.75" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -785,7 +801,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -796,7 +812,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -834,7 +850,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -869,7 +885,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -886,7 +902,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -903,7 +919,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -923,7 +939,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -943,7 +959,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -960,7 +976,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -980,7 +996,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -997,7 +1013,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -1014,7 +1030,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -1040,20 +1056,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="3" width="10.7109375" style="3"/>
-    <col min="4" max="4" width="10.7109375" style="2"/>
+    <col min="2" max="3" width="10.75" style="3"/>
+    <col min="4" max="4" width="10.75" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1064,7 +1080,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1075,7 +1091,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1113,7 +1129,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -1145,7 +1161,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -1159,7 +1175,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -1174,7 +1190,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -1186,20 +1201,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="3" width="10.7109375" style="3"/>
-    <col min="4" max="4" width="10.7109375" style="2"/>
+    <col min="2" max="3" width="10.75" style="3"/>
+    <col min="4" max="4" width="10.75" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1213,7 +1228,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1224,7 +1239,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1262,7 +1277,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -1295,7 +1310,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -1307,20 +1321,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:N6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="3" width="10.7109375" style="3"/>
-    <col min="4" max="4" width="10.7109375" style="2"/>
+    <col min="2" max="3" width="10.75" style="3"/>
+    <col min="4" max="4" width="10.75" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1331,7 +1345,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1342,7 +1356,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1380,15 +1394,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>44</v>
       </c>
       <c r="B4" s="3">
         <v>40073</v>
       </c>
+      <c r="C4" s="3">
+        <v>40075</v>
+      </c>
       <c r="D4" s="2">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -1400,7 +1417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>48</v>
       </c>
@@ -1413,23 +1430,42 @@
       <c r="E5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:14">
+      <c r="M5" s="1">
+        <v>40085</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>49</v>
       </c>
       <c r="B6" s="3">
         <v>40081</v>
       </c>
+      <c r="C6" s="3">
+        <v>40080</v>
+      </c>
       <c r="D6" s="2">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="E6">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="3">
+        <v>40086</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="E7">
         <v>3.5</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
start of merge of gps and 2-way server
</commit_message>
<xml_diff>
--- a/Documentation/WeeklyStatus_Jacob.xlsx
+++ b/Documentation/WeeklyStatus_Jacob.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="34400" windowHeight="22600" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="34400" windowHeight="22600" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="9-2-13" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="9-23-13" sheetId="4" r:id="rId4"/>
     <sheet name="9-30-13" sheetId="5" r:id="rId5"/>
     <sheet name="10-7-13" sheetId="7" r:id="rId6"/>
+    <sheet name="10-21-13" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="55">
+  <si>
+    <t>Read Android Documentation on UDP servers and using both send and receive in same app</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
   <si>
     <t>Code Android send/receive server</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -239,21 +244,13 @@
   </si>
   <si>
     <t>Project Plan 1</t>
-  </si>
-  <si>
-    <t>Read Android Documentation on UDP servers and using both send and receive in same app</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
   </numFmts>
@@ -643,14 +640,14 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1">
         <v>39995</v>
       </c>
       <c r="C1" s="1"/>
       <c r="E1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F1">
         <v>6</v>
@@ -658,56 +655,56 @@
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" t="s">
         <v>25</v>
       </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K3" t="s">
-        <v>24</v>
-      </c>
       <c r="M3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1">
         <v>39995</v>
@@ -722,16 +719,16 @@
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" t="s">
         <v>23</v>
-      </c>
-      <c r="I4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J4" t="s">
-        <v>22</v>
       </c>
       <c r="K4">
         <v>0.5</v>
@@ -745,7 +742,7 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1">
         <v>39995</v>
@@ -758,12 +755,12 @@
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1">
         <v>39995</v>
@@ -778,7 +775,7 @@
         <v>2.5</v>
       </c>
       <c r="F6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -808,67 +805,67 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B1" s="3">
         <v>40002</v>
       </c>
       <c r="E1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" t="s">
         <v>25</v>
       </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K3" t="s">
-        <v>24</v>
-      </c>
       <c r="M3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B4" s="3">
         <v>40059</v>
@@ -883,13 +880,13 @@
         <v>0.75</v>
       </c>
       <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" t="s">
         <v>23</v>
-      </c>
-      <c r="I4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J4" t="s">
-        <v>22</v>
       </c>
       <c r="K4">
         <v>0.5</v>
@@ -903,7 +900,7 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B5" s="3">
         <v>40061</v>
@@ -920,7 +917,7 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B6" s="3">
         <v>40059</v>
@@ -937,7 +934,7 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B7" s="3">
         <v>40063</v>
@@ -952,12 +949,12 @@
         <v>0.5</v>
       </c>
       <c r="F7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B8" s="3">
         <v>40063</v>
@@ -972,12 +969,12 @@
         <v>0.25</v>
       </c>
       <c r="F8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B9" s="3">
         <v>40063</v>
@@ -994,7 +991,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B10" s="3">
         <v>40061</v>
@@ -1009,12 +1006,12 @@
         <v>0.75</v>
       </c>
       <c r="F10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B11" s="3">
         <v>40063</v>
@@ -1031,7 +1028,7 @@
     </row>
     <row r="12" spans="1:14">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B12" s="3">
         <v>40063</v>
@@ -1048,7 +1045,7 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B13" s="3">
         <v>40063</v>
@@ -1087,67 +1084,67 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B1" s="3">
         <v>40002</v>
       </c>
       <c r="E1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" t="s">
         <v>25</v>
       </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K3" t="s">
-        <v>24</v>
-      </c>
       <c r="M3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B4" s="3">
         <v>40073</v>
@@ -1159,13 +1156,13 @@
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K4">
         <v>0.5</v>
@@ -1179,7 +1176,7 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B5" s="3">
         <v>40066</v>
@@ -1193,7 +1190,7 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B6" s="3">
         <v>40069</v>
@@ -1232,13 +1229,13 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B1" s="3">
         <v>40078</v>
       </c>
       <c r="E1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F1">
         <v>11</v>
@@ -1246,56 +1243,56 @@
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" t="s">
         <v>25</v>
       </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K3" t="s">
-        <v>24</v>
-      </c>
       <c r="M3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B4" s="3">
         <v>40073</v>
@@ -1307,13 +1304,13 @@
         <v>9</v>
       </c>
       <c r="H4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K4">
         <v>1</v>
@@ -1352,67 +1349,67 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B1" s="3">
         <v>40085</v>
       </c>
       <c r="E1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" t="s">
         <v>25</v>
       </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K3" t="s">
-        <v>24</v>
-      </c>
       <c r="M3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B4" s="3">
         <v>40073</v>
@@ -1435,7 +1432,7 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B5" s="3">
         <v>40079</v>
@@ -1452,7 +1449,7 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B6" s="3">
         <v>40081</v>
@@ -1469,7 +1466,7 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B7" s="3">
         <v>40086</v>
@@ -1496,7 +1493,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -1508,67 +1505,67 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B1" s="3">
         <v>40092</v>
       </c>
       <c r="E1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" t="s">
         <v>25</v>
       </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K3" t="s">
-        <v>24</v>
-      </c>
       <c r="M3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="B4" s="3">
         <v>40088</v>
@@ -1586,7 +1583,7 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B5" s="3">
         <v>40089</v>
@@ -1604,7 +1601,7 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B6" s="3">
         <v>40092</v>
@@ -1621,7 +1618,7 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B7" s="3">
         <v>40102</v>
@@ -1639,7 +1636,105 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <dimension ref="A1:N5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
+  <cols>
+    <col min="2" max="3" width="11" style="3"/>
+    <col min="4" max="4" width="11" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3">
+        <v>40106</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="M4" s="1">
+        <v>40101</v>
+      </c>
+      <c r="N4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="M5" s="1"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Updates to 2 way server, and adding new tablet app
</commit_message>
<xml_diff>
--- a/Documentation/WeeklyStatus_Jacob.xlsx
+++ b/Documentation/WeeklyStatus_Jacob.xlsx
@@ -26,7 +26,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="58">
+  <si>
+    <t>Android to Vex Comm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LinuxHowTos.org</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sockets Tutorial</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N/A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Interrupt based obstacle avoidance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sending Waypoints from tablet to phone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
   <si>
     <t>Project Report</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -232,26 +256,6 @@
   </si>
   <si>
     <t>Building a Dynamic UI with Fragments, Creating a Fragment</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Android to Vex Comm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LinuxHowTos.org</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sockets Tutorial</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>N/A</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Interrupt based obstacle avoidance</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -649,14 +653,14 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1">
         <v>39995</v>
       </c>
       <c r="C1" s="1"/>
       <c r="E1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F1">
         <v>6</v>
@@ -664,56 +668,56 @@
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="M2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="I3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="J3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="K3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="M3" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="N3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B4" s="1">
         <v>39995</v>
@@ -728,16 +732,16 @@
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="H4" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="I4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="J4" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="K4">
         <v>0.5</v>
@@ -751,7 +755,7 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B5" s="1">
         <v>39995</v>
@@ -764,12 +768,12 @@
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B6" s="1">
         <v>39995</v>
@@ -784,7 +788,7 @@
         <v>2.5</v>
       </c>
       <c r="F6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -814,67 +818,67 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B1" s="3">
         <v>40002</v>
       </c>
       <c r="E1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="M2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="I3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="J3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="K3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="M3" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="N3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B4" s="3">
         <v>40059</v>
@@ -889,13 +893,13 @@
         <v>0.75</v>
       </c>
       <c r="H4" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="I4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="J4" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="K4">
         <v>0.5</v>
@@ -909,7 +913,7 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="B5" s="3">
         <v>40061</v>
@@ -926,7 +930,7 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B6" s="3">
         <v>40059</v>
@@ -943,7 +947,7 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B7" s="3">
         <v>40063</v>
@@ -958,12 +962,12 @@
         <v>0.5</v>
       </c>
       <c r="F7" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B8" s="3">
         <v>40063</v>
@@ -978,12 +982,12 @@
         <v>0.25</v>
       </c>
       <c r="F8" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B9" s="3">
         <v>40063</v>
@@ -1000,7 +1004,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="B10" s="3">
         <v>40061</v>
@@ -1015,12 +1019,12 @@
         <v>0.75</v>
       </c>
       <c r="F10" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B11" s="3">
         <v>40063</v>
@@ -1037,7 +1041,7 @@
     </row>
     <row r="12" spans="1:14">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B12" s="3">
         <v>40063</v>
@@ -1054,7 +1058,7 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B13" s="3">
         <v>40063</v>
@@ -1093,67 +1097,67 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B1" s="3">
         <v>40002</v>
       </c>
       <c r="E1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="M2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="I3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="J3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="K3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="M3" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="N3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B4" s="3">
         <v>40073</v>
@@ -1165,13 +1169,13 @@
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="I4" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="J4" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="K4">
         <v>0.5</v>
@@ -1185,7 +1189,7 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B5" s="3">
         <v>40066</v>
@@ -1199,7 +1203,7 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B6" s="3">
         <v>40069</v>
@@ -1238,13 +1242,13 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B1" s="3">
         <v>40078</v>
       </c>
       <c r="E1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F1">
         <v>11</v>
@@ -1252,56 +1256,56 @@
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="M2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="I3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="J3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="K3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="M3" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="N3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="B4" s="3">
         <v>40073</v>
@@ -1313,13 +1317,13 @@
         <v>9</v>
       </c>
       <c r="H4" t="s">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
       <c r="J4" t="s">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="K4">
         <v>1</v>
@@ -1358,67 +1362,67 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B1" s="3">
         <v>40085</v>
       </c>
       <c r="E1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="M2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="I3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="J3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="K3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="M3" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="N3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="B4" s="3">
         <v>40073</v>
@@ -1441,7 +1445,7 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="B5" s="3">
         <v>40079</v>
@@ -1458,7 +1462,7 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B6" s="3">
         <v>40081</v>
@@ -1475,7 +1479,7 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B7" s="3">
         <v>40086</v>
@@ -1514,67 +1518,67 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B1" s="3">
         <v>40092</v>
       </c>
       <c r="E1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="M2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="I3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="J3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="K3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="M3" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="N3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B4" s="3">
         <v>40088</v>
@@ -1592,7 +1596,7 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B5" s="3">
         <v>40089</v>
@@ -1610,7 +1614,7 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B6" s="3">
         <v>40092</v>
@@ -1627,7 +1631,7 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B7" s="3">
         <v>40102</v>
@@ -1669,13 +1673,13 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B1" s="3">
         <v>40106</v>
       </c>
       <c r="E1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F1">
         <v>0.5</v>
@@ -1683,51 +1687,51 @@
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="M2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="I3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="J3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="K3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="M3" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="N3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -1754,10 +1758,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
@@ -1768,13 +1772,13 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B1" s="3">
         <v>40113</v>
       </c>
       <c r="E1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F1">
         <v>0.5</v>
@@ -1782,56 +1786,56 @@
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="M2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="I3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="J3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="K3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="M3" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="N3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B4" s="3">
         <v>40106</v>
@@ -1845,11 +1849,16 @@
       <c r="E4">
         <v>3</v>
       </c>
-      <c r="M4" s="1"/>
+      <c r="M4" s="1">
+        <v>40108</v>
+      </c>
+      <c r="N4">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B5" s="3">
         <v>40111</v>
@@ -1858,9 +1867,20 @@
         <v>0.1</v>
       </c>
       <c r="E5">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="M5" s="1"/>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Update 2 way server to use wifi based positioning and my weekly schedule
</commit_message>
<xml_diff>
--- a/Documentation/WeeklyStatus_Jacob.xlsx
+++ b/Documentation/WeeklyStatus_Jacob.xlsx
@@ -26,7 +26,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="59">
+  <si>
+    <t>Investigate ssh on android</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Write android end of vex-android communcation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Android.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N/A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Building a Dynamic UI with Fragments, Creating a Fragment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Robot Moves Straight</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
   <si>
     <t>Android to Vex Comm</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -236,26 +260,6 @@
   </si>
   <si>
     <t>Write and test sending ssh movement commands from pc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Investigate ssh on android</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Write android end of vex-android communcation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Android.com</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>N/A</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Building a Dynamic UI with Fragments, Creating a Fragment</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -653,14 +657,14 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1">
         <v>39995</v>
       </c>
       <c r="C1" s="1"/>
       <c r="E1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="F1">
         <v>6</v>
@@ -668,56 +672,56 @@
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="H2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="M2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="H3" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="I3" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="J3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="K3" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="M3" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="N3" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B4" s="1">
         <v>39995</v>
@@ -732,16 +736,16 @@
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="H4" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="I4" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="J4" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="K4">
         <v>0.5</v>
@@ -755,7 +759,7 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B5" s="1">
         <v>39995</v>
@@ -768,12 +772,12 @@
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B6" s="1">
         <v>39995</v>
@@ -788,7 +792,7 @@
         <v>2.5</v>
       </c>
       <c r="F6" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -818,67 +822,67 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B1" s="3">
         <v>40002</v>
       </c>
       <c r="E1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="H2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="M2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="H3" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="I3" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="J3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="K3" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="M3" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="N3" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B4" s="3">
         <v>40059</v>
@@ -893,13 +897,13 @@
         <v>0.75</v>
       </c>
       <c r="H4" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="I4" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="J4" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="K4">
         <v>0.5</v>
@@ -913,7 +917,7 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B5" s="3">
         <v>40061</v>
@@ -930,7 +934,7 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="B6" s="3">
         <v>40059</v>
@@ -947,7 +951,7 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B7" s="3">
         <v>40063</v>
@@ -962,12 +966,12 @@
         <v>0.5</v>
       </c>
       <c r="F7" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B8" s="3">
         <v>40063</v>
@@ -982,12 +986,12 @@
         <v>0.25</v>
       </c>
       <c r="F8" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B9" s="3">
         <v>40063</v>
@@ -1004,7 +1008,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B10" s="3">
         <v>40061</v>
@@ -1019,12 +1023,12 @@
         <v>0.75</v>
       </c>
       <c r="F10" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B11" s="3">
         <v>40063</v>
@@ -1041,7 +1045,7 @@
     </row>
     <row r="12" spans="1:14">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="B12" s="3">
         <v>40063</v>
@@ -1058,7 +1062,7 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B13" s="3">
         <v>40063</v>
@@ -1097,67 +1101,67 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B1" s="3">
         <v>40002</v>
       </c>
       <c r="E1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="H2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="M2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="H3" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="I3" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="J3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="K3" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="M3" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="N3" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B4" s="3">
         <v>40073</v>
@@ -1169,13 +1173,13 @@
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="I4" t="s">
-        <v>56</v>
+        <v>3</v>
       </c>
       <c r="J4" t="s">
-        <v>57</v>
+        <v>4</v>
       </c>
       <c r="K4">
         <v>0.5</v>
@@ -1189,7 +1193,7 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="B5" s="3">
         <v>40066</v>
@@ -1203,7 +1207,7 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>1</v>
       </c>
       <c r="B6" s="3">
         <v>40069</v>
@@ -1242,13 +1246,13 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B1" s="3">
         <v>40078</v>
       </c>
       <c r="E1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="F1">
         <v>11</v>
@@ -1256,56 +1260,56 @@
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="H2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="M2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="H3" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="I3" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="J3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="K3" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="M3" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="N3" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B4" s="3">
         <v>40073</v>
@@ -1317,13 +1321,13 @@
         <v>9</v>
       </c>
       <c r="H4" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I4" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J4" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="K4">
         <v>1</v>
@@ -1362,67 +1366,67 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B1" s="3">
         <v>40085</v>
       </c>
       <c r="E1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="H2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="M2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="H3" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="I3" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="J3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="K3" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="M3" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="N3" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B4" s="3">
         <v>40073</v>
@@ -1445,7 +1449,7 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B5" s="3">
         <v>40079</v>
@@ -1462,7 +1466,7 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B6" s="3">
         <v>40081</v>
@@ -1479,7 +1483,7 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B7" s="3">
         <v>40086</v>
@@ -1518,67 +1522,67 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B1" s="3">
         <v>40092</v>
       </c>
       <c r="E1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="H2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="M2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="H3" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="I3" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="J3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="K3" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="M3" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="N3" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3">
         <v>40088</v>
@@ -1596,7 +1600,7 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B5" s="3">
         <v>40089</v>
@@ -1614,7 +1618,7 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B6" s="3">
         <v>40092</v>
@@ -1631,7 +1635,7 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B7" s="3">
         <v>40102</v>
@@ -1673,13 +1677,13 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B1" s="3">
         <v>40106</v>
       </c>
       <c r="E1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="F1">
         <v>0.5</v>
@@ -1687,51 +1691,51 @@
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="H2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="M2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="H3" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="I3" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="J3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="K3" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="M3" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="N3" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -1758,10 +1762,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
@@ -1772,70 +1776,70 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B1" s="3">
         <v>40113</v>
       </c>
       <c r="E1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="F1">
-        <v>0.5</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="H2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="M2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="H3" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="I3" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="J3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="K3" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="M3" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="N3" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B4" s="3">
         <v>40106</v>
@@ -1858,27 +1862,47 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B5" s="3">
         <v>40111</v>
       </c>
       <c r="D5" s="2">
-        <v>0.1</v>
+        <v>0.9</v>
       </c>
       <c r="E5">
-        <v>1.5</v>
+        <v>5</v>
       </c>
       <c r="M5" s="1"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="3">
+        <v>40111</v>
+      </c>
+      <c r="C6" s="3">
+        <v>40111</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="E6">
+      <c r="B7" s="3">
+        <v>40115</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="E7">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added start of phase 3 project plan and updated weekly status
</commit_message>
<xml_diff>
--- a/Documentation/WeeklyStatus_Jacob.xlsx
+++ b/Documentation/WeeklyStatus_Jacob.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\4049dahleej\Documents\GitHub\EmbeddedSystems\Documentation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="34400" windowHeight="22600" tabRatio="500" activeTab="8"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="34395" windowHeight="22605" tabRatio="500" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="9-2-13" sheetId="1" r:id="rId1"/>
@@ -27,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="64">
   <si>
     <t>Start 3:30</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -278,17 +283,20 @@
   <si>
     <t>Replace 3-wire motors with 2-wire</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Phase 3 Plan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -659,20 +667,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -687,7 +695,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -698,7 +706,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -736,7 +744,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -774,7 +782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -792,7 +800,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>52</v>
       </c>
@@ -824,20 +832,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="3" width="11" style="3"/>
     <col min="4" max="4" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -848,7 +856,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -859,7 +867,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -897,7 +905,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -932,7 +940,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>55</v>
       </c>
@@ -949,7 +957,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -966,7 +974,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -986,7 +994,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>59</v>
       </c>
@@ -1006,7 +1014,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>61</v>
       </c>
@@ -1023,7 +1031,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>62</v>
       </c>
@@ -1043,7 +1051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -1060,7 +1068,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -1077,7 +1085,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -1103,20 +1111,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="3" width="11" style="3"/>
     <col min="4" max="4" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -1127,7 +1135,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -1138,7 +1146,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1176,7 +1184,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1208,7 +1216,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1222,7 +1230,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1248,20 +1256,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="3" width="11" style="3"/>
     <col min="4" max="4" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -1275,7 +1283,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -1286,7 +1294,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1324,7 +1332,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1368,20 +1376,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="3" width="11" style="3"/>
     <col min="4" max="4" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -1392,7 +1400,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -1403,7 +1411,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1441,7 +1449,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1464,7 +1472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1481,7 +1489,7 @@
         <v>40085</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1498,7 +1506,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -1524,20 +1532,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="3" width="11" style="3"/>
     <col min="4" max="4" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -1548,7 +1556,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -1559,7 +1567,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1597,7 +1605,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -1615,7 +1623,7 @@
       </c>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -1633,7 +1641,7 @@
       </c>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -1650,7 +1658,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1679,20 +1687,20 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="3" width="11" style="3"/>
     <col min="4" max="4" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -1706,7 +1714,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -1717,7 +1725,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1755,7 +1763,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="M4" s="1">
         <v>40101</v>
       </c>
@@ -1763,7 +1771,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="M5" s="1"/>
     </row>
   </sheetData>
@@ -1778,20 +1786,20 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="3" width="11" style="3"/>
     <col min="4" max="4" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -1805,7 +1813,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -1816,7 +1824,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1854,7 +1862,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -1877,7 +1885,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -1892,7 +1900,7 @@
       </c>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1909,7 +1917,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1935,20 +1943,20 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:N7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="3" width="11" style="3"/>
     <col min="4" max="4" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -1962,7 +1970,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -1973,7 +1981,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -2011,7 +2019,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -2034,7 +2042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -2052,7 +2060,7 @@
       </c>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -2069,7 +2077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -2084,6 +2092,20 @@
       </c>
       <c r="E7">
         <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="3">
+        <v>40121</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Continue work on project plan and tasks for phase 3
</commit_message>
<xml_diff>
--- a/Documentation/WeeklyStatus_Jacob.xlsx
+++ b/Documentation/WeeklyStatus_Jacob.xlsx
@@ -5,7 +5,7 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\4049dahleej\Documents\GitHub\EmbeddedSystems\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdahleen\Documents\GitHub\EmbeddedSystems\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -304,6 +304,7 @@
     <font>
       <sz val="8"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1947,7 +1948,7 @@
   <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2102,10 +2103,10 @@
         <v>40121</v>
       </c>
       <c r="D8" s="2">
-        <v>0.3</v>
+        <v>0.9</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>2.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>